<commit_message>
[FIX] Corrección de navegación y creación de archivos
</commit_message>
<xml_diff>
--- a/jugadores.xlsx
+++ b/jugadores.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,19 +428,19 @@
         <v>clubAlt</v>
       </c>
       <c r="I1" t="str">
+        <v>valorCarrera</v>
+      </c>
+      <c r="J1" t="str">
+        <v>ultimaRevision</v>
+      </c>
+      <c r="K1" t="str">
         <v>valorMercado</v>
       </c>
-      <c r="J1" t="str">
+      <c r="L1" t="str">
         <v>nacionalidad2Alt</v>
       </c>
-      <c r="K1" t="str">
+      <c r="M1" t="str">
         <v>nacionalidad2</v>
-      </c>
-      <c r="L1" t="str">
-        <v>valorCarrera</v>
-      </c>
-      <c r="M1" t="str">
-        <v>ultimaRevision</v>
       </c>
     </row>
     <row r="2">
@@ -469,6 +469,12 @@
         <v>Manchester City</v>
       </c>
       <c r="I2" t="str">
+        <v>200,00 mill. €</v>
+      </c>
+      <c r="J2" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K2" t="str">
         <v>180,00 mill. €</v>
       </c>
     </row>
@@ -501,80 +507,98 @@
         <v>150,00 mill. €</v>
       </c>
       <c r="J3" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K3" t="str">
+        <v>150,00 mill. €</v>
+      </c>
+      <c r="L3" t="str">
         <v>Nigeria</v>
       </c>
-      <c r="K3" t="str">
+      <c r="M3" t="str">
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Alexander Isak</v>
+        <v>Declan Rice</v>
       </c>
       <c r="B4" t="str">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" t="str">
-        <v>Delantero centro</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D4" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/349066-1680791339.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/357662-1687962936.jpg?lm=1</v>
       </c>
       <c r="E4" t="str">
-        <v>Suecia</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F4" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G4" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H4" t="str">
-        <v>Newcastle United</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I4" t="str">
         <v>120,00 mill. €</v>
       </c>
       <c r="J4" t="str">
-        <v>Eritrea</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K4" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/46.png?lm=1520611569</v>
+        <v>120,00 mill. €</v>
+      </c>
+      <c r="L4" t="str">
+        <v>Irlanda</v>
+      </c>
+      <c r="M4" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/72.png?lm=1520611569</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Declan Rice</v>
+        <v>Alexander Isak</v>
       </c>
       <c r="B5" t="str">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="str">
-        <v>Mediocentro</v>
+        <v>Delantero centro</v>
       </c>
       <c r="D5" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/357662-1687962936.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/349066-1680791339.jpg?lm=1</v>
       </c>
       <c r="E5" t="str">
-        <v>Inglaterra</v>
+        <v>Suecia</v>
       </c>
       <c r="F5" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
       </c>
       <c r="G5" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
       </c>
       <c r="H5" t="str">
-        <v>Arsenal FC</v>
+        <v>Newcastle United</v>
       </c>
       <c r="I5" t="str">
         <v>120,00 mill. €</v>
       </c>
       <c r="J5" t="str">
-        <v>Irlanda</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K5" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/72.png?lm=1520611569</v>
+        <v>120,00 mill. €</v>
+      </c>
+      <c r="L5" t="str">
+        <v>Eritrea</v>
+      </c>
+      <c r="M5" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/46.png?lm=1520611569</v>
       </c>
     </row>
     <row r="6">
@@ -603,6 +627,12 @@
         <v>Chelsea FC</v>
       </c>
       <c r="I6" t="str">
+        <v>130,00 mill. €</v>
+      </c>
+      <c r="J6" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K6" t="str">
         <v>120,00 mill. €</v>
       </c>
     </row>
@@ -632,71 +662,89 @@
         <v>Manchester City</v>
       </c>
       <c r="I7" t="str">
+        <v>130,00 mill. €</v>
+      </c>
+      <c r="J7" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K7" t="str">
         <v>110,00 mill. €</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Phil Foden</v>
+        <v>Alexis Mac Allister</v>
       </c>
       <c r="B8" t="str">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="str">
-        <v>Extremo derecho</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D8" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/406635-1668524492.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/534033-1669835342.jpg?lm=1</v>
       </c>
       <c r="E8" t="str">
-        <v>Inglaterra</v>
+        <v>Argentina</v>
       </c>
       <c r="F8" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
       </c>
       <c r="G8" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
       </c>
       <c r="H8" t="str">
-        <v>Manchester City</v>
+        <v>Liverpool FC</v>
       </c>
       <c r="I8" t="str">
         <v>100,00 mill. €</v>
       </c>
+      <c r="J8" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K8" t="str">
+        <v>100,00 mill. €</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Italia</v>
+      </c>
+      <c r="M8" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Alexis Mac Allister</v>
+        <v>Phil Foden</v>
       </c>
       <c r="B9" t="str">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="str">
-        <v>Mediocentro</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D9" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/534033-1669835342.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/406635-1668524492.jpg?lm=1</v>
       </c>
       <c r="E9" t="str">
-        <v>Argentina</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F9" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G9" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H9" t="str">
-        <v>Liverpool FC</v>
+        <v>Manchester City</v>
       </c>
       <c r="I9" t="str">
+        <v>150,00 mill. €</v>
+      </c>
+      <c r="J9" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K9" t="str">
         <v>100,00 mill. €</v>
-      </c>
-      <c r="J9" t="str">
-        <v>Italia</v>
-      </c>
-      <c r="K9" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
       </c>
     </row>
     <row r="10">
@@ -727,6 +775,12 @@
       <c r="I10" t="str">
         <v>90,00 mill. €</v>
       </c>
+      <c r="J10" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K10" t="str">
+        <v>90,00 mill. €</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -754,77 +808,95 @@
         <v>Arsenal FC</v>
       </c>
       <c r="I11" t="str">
+        <v>110,00 mill. €</v>
+      </c>
+      <c r="J11" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K11" t="str">
         <v>85,00 mill. €</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>William Saliba</v>
+        <v>Bruno Guimarães</v>
       </c>
       <c r="B12" t="str">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C12" t="str">
-        <v>Defensa central</v>
+        <v>Pivote</v>
       </c>
       <c r="D12" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/495666-1718697201.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/520624-1668522672.jpg?lm=1</v>
       </c>
       <c r="E12" t="str">
-        <v>Francia</v>
+        <v>Brasil</v>
       </c>
       <c r="F12" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
       <c r="G12" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
       </c>
       <c r="H12" t="str">
-        <v>Arsenal FC</v>
+        <v>Newcastle United</v>
       </c>
       <c r="I12" t="str">
+        <v>85,00 mill. €</v>
+      </c>
+      <c r="J12" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K12" t="str">
         <v>80,00 mill. €</v>
       </c>
-      <c r="J12" t="str">
-        <v>Camerún</v>
-      </c>
-      <c r="K12" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
+      <c r="L12" t="str">
+        <v>España</v>
+      </c>
+      <c r="M12" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Bruno Guimarães</v>
+        <v>William Saliba</v>
       </c>
       <c r="B13" t="str">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" t="str">
-        <v>Pivote</v>
+        <v>Defensa central</v>
       </c>
       <c r="D13" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/520624-1668522672.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/495666-1718697201.jpg?lm=1</v>
       </c>
       <c r="E13" t="str">
-        <v>Brasil</v>
+        <v>Francia</v>
       </c>
       <c r="F13" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
       </c>
       <c r="G13" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H13" t="str">
-        <v>Newcastle United</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I13" t="str">
         <v>80,00 mill. €</v>
       </c>
       <c r="J13" t="str">
-        <v>España</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K13" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
+        <v>80,00 mill. €</v>
+      </c>
+      <c r="L13" t="str">
+        <v>Camerún</v>
+      </c>
+      <c r="M13" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
       </c>
     </row>
     <row r="14">
@@ -855,6 +927,12 @@
       <c r="I14" t="str">
         <v>80,00 mill. €</v>
       </c>
+      <c r="J14" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K14" t="str">
+        <v>80,00 mill. €</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -884,6 +962,12 @@
       <c r="I15" t="str">
         <v>75,00 mill. €</v>
       </c>
+      <c r="J15" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K15" t="str">
+        <v>75,00 mill. €</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -914,67 +998,85 @@
         <v>75,00 mill. €</v>
       </c>
       <c r="J16" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K16" t="str">
+        <v>75,00 mill. €</v>
+      </c>
+      <c r="L16" t="str">
         <v>Canadá</v>
       </c>
-      <c r="K16" t="str">
+      <c r="M16" t="str">
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/80.png?lm=1520611569</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Josko Gvardiol</v>
+        <v>Enzo Fernández</v>
       </c>
       <c r="B17" t="str">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="str">
-        <v>Lateral izquierdo</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D17" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/475959-1713391602.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/648195-1669894717.jpg?lm=1</v>
       </c>
       <c r="E17" t="str">
-        <v>Croacia</v>
+        <v>Argentina</v>
       </c>
       <c r="F17" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/37.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
       </c>
       <c r="G17" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H17" t="str">
-        <v>Manchester City</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I17" t="str">
+        <v>85,00 mill. €</v>
+      </c>
+      <c r="J17" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K17" t="str">
         <v>75,00 mill. €</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Enzo Fernández</v>
+        <v>Josko Gvardiol</v>
       </c>
       <c r="B18" t="str">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="str">
-        <v>Mediocentro</v>
+        <v>Lateral izquierdo</v>
       </c>
       <c r="D18" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/648195-1669894717.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/475959-1713391602.jpg?lm=1</v>
       </c>
       <c r="E18" t="str">
-        <v>Argentina</v>
+        <v>Croacia</v>
       </c>
       <c r="F18" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/37.png?lm=1520611569</v>
       </c>
       <c r="G18" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H18" t="str">
-        <v>Chelsea FC</v>
+        <v>Manchester City</v>
       </c>
       <c r="I18" t="str">
+        <v>80,00 mill. €</v>
+      </c>
+      <c r="J18" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K18" t="str">
         <v>75,00 mill. €</v>
       </c>
     </row>
@@ -1007,30 +1109,36 @@
         <v>75,00 mill. €</v>
       </c>
       <c r="J19" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K19" t="str">
+        <v>75,00 mill. €</v>
+      </c>
+      <c r="L19" t="str">
         <v>Surinam</v>
       </c>
-      <c r="K19" t="str">
+      <c r="M19" t="str">
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/161.png?lm=1520611569</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Cody Gakpo</v>
+        <v>Luis Díaz</v>
       </c>
       <c r="B20" t="str">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" t="str">
         <v>Extremo izquierdo</v>
       </c>
       <c r="D20" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/434675-1682690965.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/480692-1697903145.jpg?lm=1</v>
       </c>
       <c r="E20" t="str">
-        <v>Países Bajos</v>
+        <v>Colombia</v>
       </c>
       <c r="F20" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/83.png?lm=1520611569</v>
       </c>
       <c r="G20" t="str">
         <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
@@ -1039,33 +1147,33 @@
         <v>Liverpool FC</v>
       </c>
       <c r="I20" t="str">
+        <v>85,00 mill. €</v>
+      </c>
+      <c r="J20" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K20" t="str">
         <v>70,00 mill. €</v>
-      </c>
-      <c r="J20" t="str">
-        <v>Togo</v>
-      </c>
-      <c r="K20" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/168.png?lm=1520611569</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Luis Díaz</v>
+        <v>Cody Gakpo</v>
       </c>
       <c r="B21" t="str">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" t="str">
         <v>Extremo izquierdo</v>
       </c>
       <c r="D21" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/480692-1697903145.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/434675-1682690965.jpg?lm=1</v>
       </c>
       <c r="E21" t="str">
-        <v>Colombia</v>
+        <v>Países Bajos</v>
       </c>
       <c r="F21" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/83.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
       </c>
       <c r="G21" t="str">
         <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
@@ -1076,325 +1184,481 @@
       <c r="I21" t="str">
         <v>70,00 mill. €</v>
       </c>
+      <c r="J21" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K21" t="str">
+        <v>70,00 mill. €</v>
+      </c>
+      <c r="L21" t="str">
+        <v>Togo</v>
+      </c>
+      <c r="M21" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/168.png?lm=1520611569</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Rúben Dias</v>
+        <v>Kai Havertz</v>
       </c>
       <c r="B22" t="str">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" t="str">
-        <v>Defensa central</v>
+        <v>Delantero centro</v>
       </c>
       <c r="D22" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/258004-1684921271.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/309400-1683903902.jpg?lm=1</v>
       </c>
       <c r="E22" t="str">
-        <v>Portugal</v>
+        <v>Alemania</v>
       </c>
       <c r="F22" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/40.png?lm=1520612525</v>
       </c>
       <c r="G22" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H22" t="str">
-        <v>Manchester City</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I22" t="str">
+        <v>90,00 mill. €</v>
+      </c>
+      <c r="J22" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K22" t="str">
         <v>65,00 mill. €</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Kai Havertz</v>
+        <v>Anthony Gordon</v>
       </c>
       <c r="B23" t="str">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" t="str">
-        <v>Delantero centro</v>
+        <v>Extremo izquierdo</v>
       </c>
       <c r="D23" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/309400-1683903902.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/503733-1660588736.jpg?lm=1</v>
       </c>
       <c r="E23" t="str">
-        <v>Alemania</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F23" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/40.png?lm=1520612525</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G23" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
       </c>
       <c r="H23" t="str">
-        <v>Arsenal FC</v>
+        <v>Newcastle United</v>
       </c>
       <c r="I23" t="str">
         <v>65,00 mill. €</v>
       </c>
+      <c r="J23" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K23" t="str">
+        <v>65,00 mill. €</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Anthony Gordon</v>
+        <v>Rúben Dias</v>
       </c>
       <c r="B24" t="str">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C24" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Defensa central</v>
       </c>
       <c r="D24" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/503733-1660588736.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/258004-1684921271.jpg?lm=1</v>
       </c>
       <c r="E24" t="str">
-        <v>Inglaterra</v>
+        <v>Portugal</v>
       </c>
       <c r="F24" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
       </c>
       <c r="G24" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H24" t="str">
-        <v>Newcastle United</v>
+        <v>Manchester City</v>
       </c>
       <c r="I24" t="str">
+        <v>80,00 mill. €</v>
+      </c>
+      <c r="J24" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K24" t="str">
         <v>65,00 mill. €</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Sandro Tonali</v>
+        <v>Tijjani Reijnders</v>
       </c>
       <c r="B25" t="str">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" t="str">
         <v>Mediocentro</v>
       </c>
       <c r="D25" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/397033-1688389270.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/460939-1676466080.jpg?lm=1</v>
       </c>
       <c r="E25" t="str">
-        <v>Italia</v>
+        <v>Países Bajos</v>
       </c>
       <c r="F25" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
       </c>
       <c r="G25" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H25" t="str">
-        <v>Newcastle United</v>
+        <v>Manchester City</v>
       </c>
       <c r="I25" t="str">
         <v>60,00 mill. €</v>
       </c>
+      <c r="J25" t="str">
+        <v>17/06/2025</v>
+      </c>
+      <c r="K25" t="str">
+        <v>60,00 mill. €</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Tijjani Reijnders</v>
+        <v>Matheus Cunha</v>
       </c>
       <c r="B26" t="str">
         <v>26</v>
       </c>
       <c r="C26" t="str">
-        <v>Mediocentro</v>
+        <v>Mediapunta</v>
       </c>
       <c r="D26" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/460939-1676466080.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/517894-1696599737.jpg?lm=1</v>
       </c>
       <c r="E26" t="str">
-        <v>Países Bajos</v>
+        <v>Brasil</v>
       </c>
       <c r="F26" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
       <c r="G26" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/543.png?lm=1467496784</v>
       </c>
       <c r="H26" t="str">
-        <v>Manchester City</v>
+        <v>Wolverhampton Wanderers</v>
       </c>
       <c r="I26" t="str">
         <v>60,00 mill. €</v>
       </c>
+      <c r="J26" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K26" t="str">
+        <v>60,00 mill. €</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Joe Whitworth</v>
+        <v>Sandro Tonali</v>
+      </c>
+      <c r="B27" t="str">
+        <v>25</v>
       </c>
       <c r="C27" t="str">
-        <v>Portero</v>
+        <v>Mediocentro</v>
+      </c>
+      <c r="D27" t="str">
+        <v>https://img.a.transfermarkt.technology/portrait/medium/397033-1688389270.jpg?lm=1</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Italia</v>
+      </c>
+      <c r="F27" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
       </c>
       <c r="G27" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/873.png?lm=1457723287</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
       </c>
       <c r="H27" t="str">
-        <v>Crystal Palace</v>
+        <v>Newcastle United</v>
       </c>
       <c r="I27" t="str">
-        <v>1,70 mill. €</v>
+        <v>60,00 mill. €</v>
+      </c>
+      <c r="J27" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K27" t="str">
+        <v>60,00 mill. €</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Tyler Bindon</v>
+        <v>Ibrahima Konaté</v>
+      </c>
+      <c r="B28" t="str">
+        <v>26</v>
       </c>
       <c r="C28" t="str">
         <v>Defensa central</v>
       </c>
+      <c r="D28" t="str">
+        <v>https://img.a.transfermarkt.technology/portrait/medium/357119-1669190550.jpg?lm=1</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Francia</v>
+      </c>
+      <c r="F28" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
+      </c>
       <c r="G28" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/703.png?lm=1598890289</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
       </c>
       <c r="H28" t="str">
-        <v>Nottingham Forest</v>
+        <v>Liverpool FC</v>
       </c>
       <c r="I28" t="str">
-        <v>1,20 mill. €</v>
+        <v>60,00 mill. €</v>
+      </c>
+      <c r="J28" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K28" t="str">
+        <v>60,00 mill. €</v>
+      </c>
+      <c r="L28" t="str">
+        <v>Malí</v>
+      </c>
+      <c r="M28" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/105.png?lm=1520611569</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Joe Hodge</v>
+        <v>Jurrien Timber</v>
+      </c>
+      <c r="B29" t="str">
+        <v>24</v>
       </c>
       <c r="C29" t="str">
-        <v>Pivote</v>
+        <v>Lateral derecho</v>
+      </c>
+      <c r="D29" t="str">
+        <v>https://img.a.transfermarkt.technology/portrait/medium/420243-1702413077.jpg?lm=1</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Países Bajos</v>
+      </c>
+      <c r="F29" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
       </c>
       <c r="G29" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/543.png?lm=1467496784</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H29" t="str">
-        <v>Wolverhampton Wanderers</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I29" t="str">
-        <v>1,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J29" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K29" t="str">
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="L29" t="str">
+        <v>Curazao</v>
+      </c>
+      <c r="M29" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/260.png?lm=1520611569</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Chem Campbell</v>
+        <v>Eberechi Eze</v>
+      </c>
+      <c r="B30" t="str">
+        <v>26</v>
       </c>
       <c r="C30" t="str">
         <v>Mediocentro ofensivo</v>
       </c>
+      <c r="D30" t="str">
+        <v>https://img.a.transfermarkt.technology/portrait/medium/479999-1678466922.jpg?lm=1</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Inglaterra</v>
+      </c>
+      <c r="F30" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+      </c>
       <c r="G30" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/543.png?lm=1467496784</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/873.png?lm=1457723287</v>
       </c>
       <c r="H30" t="str">
-        <v>Wolverhampton Wanderers</v>
+        <v>Crystal Palace</v>
       </c>
       <c r="I30" t="str">
-        <v>900 mil €</v>
+        <v>60,00 mill. €</v>
+      </c>
+      <c r="J30" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K30" t="str">
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="L30" t="str">
+        <v>Nigeria</v>
+      </c>
+      <c r="M30" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Daniel Gore</v>
+        <v>Gabriel Martinelli</v>
+      </c>
+      <c r="B31" t="str">
+        <v>24</v>
       </c>
       <c r="C31" t="str">
-        <v>Mediocentro</v>
+        <v>Extremo izquierdo</v>
+      </c>
+      <c r="D31" t="str">
+        <v>https://img.a.transfermarkt.technology/portrait/medium/655488-1682689091.jpg?lm=1</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Brasil</v>
+      </c>
+      <c r="F31" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
       <c r="G31" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H31" t="str">
-        <v>Manchester United</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I31" t="str">
-        <v>800 mil €</v>
+        <v>85,00 mill. €</v>
+      </c>
+      <c r="J31" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K31" t="str">
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="L31" t="str">
+        <v>Italia</v>
+      </c>
+      <c r="M31" t="str">
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Erling Haaland</v>
+        <v>Ethan Nwaneri</v>
       </c>
       <c r="B32" t="str">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C32" t="str">
-        <v>Delantero centro</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D32" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/418560-1709108116.png?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/890719-1730794927.jpg?lm=1</v>
       </c>
       <c r="E32" t="str">
-        <v>Noruega</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F32" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/125.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G32" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H32" t="str">
-        <v>Manchester City</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I32" t="str">
-        <v>180,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J32" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K32" t="str">
+        <v>55,00 mill. €</v>
       </c>
       <c r="L32" t="str">
-        <v>200,00 mill. €</v>
+        <v>Nigeria</v>
       </c>
       <c r="M32" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Bukayo Saka</v>
+        <v>Murillo</v>
       </c>
       <c r="B33" t="str">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" t="str">
-        <v>Extremo derecho</v>
+        <v>Defensa central</v>
       </c>
       <c r="D33" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/433177-1684155052.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/1005649-1709159139.jpg?lm=1</v>
       </c>
       <c r="E33" t="str">
-        <v>Inglaterra</v>
+        <v>Brasil</v>
       </c>
       <c r="F33" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
       <c r="G33" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/703.png?lm=1598890289</v>
       </c>
       <c r="H33" t="str">
-        <v>Arsenal FC</v>
+        <v>Nottingham Forest</v>
       </c>
       <c r="I33" t="str">
-        <v>150,00 mill. €</v>
+        <v>55,00 mill. €</v>
       </c>
       <c r="J33" t="str">
-        <v>Nigeria</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K33" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
-      </c>
-      <c r="L33" t="str">
-        <v>150,00 mill. €</v>
-      </c>
-      <c r="M33" t="str">
-        <v>30/05/2025</v>
+        <v>55,00 mill. €</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Declan Rice</v>
+        <v>Morgan Rogers</v>
       </c>
       <c r="B34" t="str">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C34" t="str">
-        <v>Mediocentro</v>
+        <v>Mediocentro ofensivo</v>
       </c>
       <c r="D34" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/357662-1687962936.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/503743-1706786450.jpg?lm=1</v>
       </c>
       <c r="E34" t="str">
         <v>Inglaterra</v>
@@ -1403,150 +1667,150 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G34" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/405.png?lm=1717155982</v>
       </c>
       <c r="H34" t="str">
-        <v>Arsenal FC</v>
+        <v>Aston Villa</v>
       </c>
       <c r="I34" t="str">
-        <v>120,00 mill. €</v>
+        <v>55,00 mill. €</v>
       </c>
       <c r="J34" t="str">
-        <v>Irlanda</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K34" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/72.png?lm=1520611569</v>
-      </c>
-      <c r="L34" t="str">
-        <v>120,00 mill. €</v>
-      </c>
-      <c r="M34" t="str">
-        <v>30/05/2025</v>
+        <v>55,00 mill. €</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Alexander Isak</v>
+        <v>Levi Colwill</v>
       </c>
       <c r="B35" t="str">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C35" t="str">
-        <v>Delantero centro</v>
+        <v>Defensa central</v>
       </c>
       <c r="D35" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/349066-1680791339.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/614258-1694614507.jpg?lm=1</v>
       </c>
       <c r="E35" t="str">
-        <v>Suecia</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F35" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G35" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H35" t="str">
-        <v>Newcastle United</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I35" t="str">
-        <v>120,00 mill. €</v>
+        <v>55,00 mill. €</v>
       </c>
       <c r="J35" t="str">
-        <v>Eritrea</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K35" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/46.png?lm=1520611569</v>
-      </c>
-      <c r="L35" t="str">
-        <v>120,00 mill. €</v>
-      </c>
-      <c r="M35" t="str">
-        <v>30/05/2025</v>
+        <v>55,00 mill. €</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Cole Palmer</v>
+        <v>Bryan Mbeumo</v>
       </c>
       <c r="B36" t="str">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C36" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D36" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/568177-1712320986.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/413039-1668505084.jpg?lm=1</v>
       </c>
       <c r="E36" t="str">
-        <v>Inglaterra</v>
+        <v>Camerún</v>
       </c>
       <c r="F36" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
       </c>
       <c r="G36" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/1148.png?lm=1625150543</v>
       </c>
       <c r="H36" t="str">
-        <v>Chelsea FC</v>
+        <v>Brentford FC</v>
       </c>
       <c r="I36" t="str">
-        <v>120,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J36" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K36" t="str">
+        <v>55,00 mill. €</v>
       </c>
       <c r="L36" t="str">
-        <v>130,00 mill. €</v>
+        <v>Francia</v>
       </c>
       <c r="M36" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Rodri</v>
+        <v>Leny Yoro</v>
       </c>
       <c r="B37" t="str">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C37" t="str">
-        <v>Pivote</v>
+        <v>Defensa central</v>
       </c>
       <c r="D37" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/357565-1682587890.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/923831-1747857948.jpg?lm=1</v>
       </c>
       <c r="E37" t="str">
-        <v>España</v>
+        <v>Francia</v>
       </c>
       <c r="F37" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
       </c>
       <c r="G37" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H37" t="str">
-        <v>Manchester City</v>
+        <v>Manchester United</v>
       </c>
       <c r="I37" t="str">
-        <v>110,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J37" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K37" t="str">
+        <v>55,00 mill. €</v>
       </c>
       <c r="L37" t="str">
-        <v>130,00 mill. €</v>
+        <v>Costa de Marfil</v>
       </c>
       <c r="M37" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/38.png?lm=1520611569</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Alexis Mac Allister</v>
+        <v>Cristian Romero</v>
       </c>
       <c r="B38" t="str">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C38" t="str">
-        <v>Mediocentro</v>
+        <v>Defensa central</v>
       </c>
       <c r="D38" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/534033-1669835342.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/355915-1665609429.jpg?lm=1</v>
       </c>
       <c r="E38" t="str">
         <v>Argentina</v>
@@ -1555,176 +1819,176 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
       </c>
       <c r="G38" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H38" t="str">
-        <v>Liverpool FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I38" t="str">
-        <v>100,00 mill. €</v>
+        <v>65,00 mill. €</v>
       </c>
       <c r="J38" t="str">
-        <v>Italia</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K38" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
-      </c>
-      <c r="L38" t="str">
-        <v>100,00 mill. €</v>
-      </c>
-      <c r="M38" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Phil Foden</v>
+        <v>João Pedro</v>
       </c>
       <c r="B39" t="str">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C39" t="str">
-        <v>Extremo derecho</v>
+        <v>Delantero centro</v>
       </c>
       <c r="D39" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/406635-1668524492.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/626724-1724792744.jpg?lm=1</v>
       </c>
       <c r="E39" t="str">
-        <v>Inglaterra</v>
+        <v>Brasil</v>
       </c>
       <c r="F39" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
       <c r="G39" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/1237.png?lm=1492718902</v>
       </c>
       <c r="H39" t="str">
-        <v>Manchester City</v>
+        <v>Brighton &amp; Hove Albion</v>
       </c>
       <c r="I39" t="str">
-        <v>100,00 mill. €</v>
-      </c>
-      <c r="L39" t="str">
-        <v>150,00 mill. €</v>
-      </c>
-      <c r="M39" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
+      </c>
+      <c r="J39" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K39" t="str">
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Moisés Caicedo</v>
+        <v>Bruno Fernandes</v>
       </c>
       <c r="B40" t="str">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C40" t="str">
-        <v>Pivote</v>
+        <v>Mediocentro ofensivo</v>
       </c>
       <c r="D40" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/687626-1660729724.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/240306-1683882766.jpg?lm=1</v>
       </c>
       <c r="E40" t="str">
-        <v>Ecuador</v>
+        <v>Portugal</v>
       </c>
       <c r="F40" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/44.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
       </c>
       <c r="G40" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H40" t="str">
-        <v>Chelsea FC</v>
+        <v>Manchester United</v>
       </c>
       <c r="I40" t="str">
         <v>90,00 mill. €</v>
       </c>
-      <c r="L40" t="str">
-        <v>90,00 mill. €</v>
-      </c>
-      <c r="M40" t="str">
-        <v>30/05/2025</v>
+      <c r="J40" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K40" t="str">
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Martin Ødegaard</v>
+        <v>Dejan Kulusevski</v>
       </c>
       <c r="B41" t="str">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" t="str">
         <v>Mediocentro ofensivo</v>
       </c>
       <c r="D41" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/316264-1678877651.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/431755-1684943454.jpg?lm=1</v>
       </c>
       <c r="E41" t="str">
-        <v>Noruega</v>
+        <v>Suecia</v>
       </c>
       <c r="F41" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/125.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
       </c>
       <c r="G41" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H41" t="str">
-        <v>Arsenal FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I41" t="str">
-        <v>85,00 mill. €</v>
+        <v>60,00 mill. €</v>
+      </c>
+      <c r="J41" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K41" t="str">
+        <v>50,00 mill. €</v>
       </c>
       <c r="L41" t="str">
-        <v>110,00 mill. €</v>
+        <v>Macedonia del Norte</v>
       </c>
       <c r="M41" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/100.png?lm=1520611569</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Bruno Guimarães</v>
+        <v>Jérémy Doku</v>
       </c>
       <c r="B42" t="str">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C42" t="str">
-        <v>Pivote</v>
+        <v>Extremo izquierdo</v>
       </c>
       <c r="D42" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/520624-1668522672.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/486049-1743670159.jpg?lm=1</v>
       </c>
       <c r="E42" t="str">
-        <v>Brasil</v>
+        <v>Bélgica</v>
       </c>
       <c r="F42" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/19.png?lm=1520611569</v>
       </c>
       <c r="G42" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H42" t="str">
-        <v>Newcastle United</v>
+        <v>Manchester City</v>
       </c>
       <c r="I42" t="str">
-        <v>80,00 mill. €</v>
+        <v>65,00 mill. €</v>
       </c>
       <c r="J42" t="str">
-        <v>España</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K42" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
+        <v>50,00 mill. €</v>
       </c>
       <c r="L42" t="str">
-        <v>85,00 mill. €</v>
+        <v>Ghana</v>
       </c>
       <c r="M42" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/54.png?lm=1520611569</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>William Saliba</v>
+        <v>Micky van de Ven</v>
       </c>
       <c r="B43" t="str">
         <v>24</v>
@@ -1733,118 +1997,124 @@
         <v>Defensa central</v>
       </c>
       <c r="D43" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/495666-1718697201.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/557459-1744313600.jpg?lm=1</v>
       </c>
       <c r="E43" t="str">
-        <v>Francia</v>
+        <v>Países Bajos</v>
       </c>
       <c r="F43" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
       </c>
       <c r="G43" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H43" t="str">
-        <v>Arsenal FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I43" t="str">
-        <v>80,00 mill. €</v>
+        <v>55,00 mill. €</v>
       </c>
       <c r="J43" t="str">
-        <v>Camerún</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K43" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
-      </c>
-      <c r="L43" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="M43" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Dominik Szoboszlai</v>
+        <v>Marcus Rashford</v>
       </c>
       <c r="B44" t="str">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C44" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Extremo izquierdo</v>
       </c>
       <c r="D44" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/451276-1700209677.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/258923-1674473054.jpg?lm=1</v>
       </c>
       <c r="E44" t="str">
-        <v>Hungría</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F44" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/178.png?lm=1521635893</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G44" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/405.png?lm=1717155982</v>
       </c>
       <c r="H44" t="str">
-        <v>Liverpool FC</v>
+        <v>Aston Villa</v>
       </c>
       <c r="I44" t="str">
-        <v>80,00 mill. €</v>
+        <v>85,00 mill. €</v>
+      </c>
+      <c r="J44" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K44" t="str">
+        <v>50,00 mill. €</v>
       </c>
       <c r="L44" t="str">
-        <v>80,00 mill. €</v>
+        <v>San Cristóbal y Nieves</v>
       </c>
       <c r="M44" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/225.png?lm=1520611569</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Gabriel Magalhães</v>
+        <v>Nicolas Jackson</v>
       </c>
       <c r="B45" t="str">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C45" t="str">
-        <v>Defensa central</v>
+        <v>Delantero centro</v>
       </c>
       <c r="D45" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/435338-1684162833.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/776890-1726227971.jpg?lm=1</v>
       </c>
       <c r="E45" t="str">
-        <v>Brasil</v>
+        <v>Senegal</v>
       </c>
       <c r="F45" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/149.png?lm=1520611569</v>
       </c>
       <c r="G45" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H45" t="str">
-        <v>Arsenal FC</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I45" t="str">
-        <v>75,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J45" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K45" t="str">
+        <v>50,00 mill. €</v>
       </c>
       <c r="L45" t="str">
-        <v>75,00 mill. €</v>
+        <v>Gambia</v>
       </c>
       <c r="M45" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/52.png?lm=1520611569</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Omar Marmoush</v>
+        <v>Mohamed Salah</v>
       </c>
       <c r="B46" t="str">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C46" t="str">
-        <v>Delantero centro</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D46" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/445939-1747656490.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/148455-1727337594.jpg?lm=1</v>
       </c>
       <c r="E46" t="str">
         <v>Egipto</v>
@@ -1853,261 +2123,261 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/2.png?lm=1520611569</v>
       </c>
       <c r="G46" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
       </c>
       <c r="H46" t="str">
-        <v>Manchester City</v>
+        <v>Liverpool FC</v>
       </c>
       <c r="I46" t="str">
-        <v>75,00 mill. €</v>
+        <v>150,00 mill. €</v>
       </c>
       <c r="J46" t="str">
-        <v>Canadá</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K46" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/80.png?lm=1520611569</v>
-      </c>
-      <c r="L46" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="M46" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Enzo Fernández</v>
+        <v>Amadou Onana</v>
       </c>
       <c r="B47" t="str">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47" t="str">
-        <v>Mediocentro</v>
+        <v>Pivote</v>
       </c>
       <c r="D47" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/648195-1669894717.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/485706-1718697649.jpg?lm=1</v>
       </c>
       <c r="E47" t="str">
-        <v>Argentina</v>
+        <v>Bélgica</v>
       </c>
       <c r="F47" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/19.png?lm=1520611569</v>
       </c>
       <c r="G47" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/405.png?lm=1717155982</v>
       </c>
       <c r="H47" t="str">
-        <v>Chelsea FC</v>
+        <v>Aston Villa</v>
       </c>
       <c r="I47" t="str">
-        <v>75,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J47" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K47" t="str">
+        <v>50,00 mill. €</v>
       </c>
       <c r="L47" t="str">
-        <v>85,00 mill. €</v>
+        <v>Senegal</v>
       </c>
       <c r="M47" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/149.png?lm=1520611569</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Josko Gvardiol</v>
+        <v>Morgan Gibbs-White</v>
       </c>
       <c r="B48" t="str">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C48" t="str">
-        <v>Lateral izquierdo</v>
+        <v>Mediocentro ofensivo</v>
       </c>
       <c r="D48" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/475959-1713391602.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/429014-1687975822.jpg?lm=1</v>
       </c>
       <c r="E48" t="str">
-        <v>Croacia</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F48" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/37.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G48" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/703.png?lm=1598890289</v>
       </c>
       <c r="H48" t="str">
-        <v>Manchester City</v>
+        <v>Nottingham Forest</v>
       </c>
       <c r="I48" t="str">
-        <v>75,00 mill. €</v>
+        <v>50,00 mill. €</v>
+      </c>
+      <c r="J48" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K48" t="str">
+        <v>50,00 mill. €</v>
       </c>
       <c r="L48" t="str">
-        <v>80,00 mill. €</v>
+        <v>Jamaica</v>
       </c>
       <c r="M48" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/76.png?lm=1520611569</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Ryan Gravenberch</v>
+        <v>Pedro Neto</v>
       </c>
       <c r="B49" t="str">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C49" t="str">
-        <v>Pivote</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D49" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/478573-1718097194.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/487465-1709158892.jpg?lm=1</v>
       </c>
       <c r="E49" t="str">
-        <v>Países Bajos</v>
+        <v>Portugal</v>
       </c>
       <c r="F49" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
       </c>
       <c r="G49" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H49" t="str">
-        <v>Liverpool FC</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I49" t="str">
-        <v>75,00 mill. €</v>
+        <v>55,00 mill. €</v>
       </c>
       <c r="J49" t="str">
-        <v>Surinam</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K49" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/161.png?lm=1520611569</v>
-      </c>
-      <c r="L49" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="M49" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Luis Díaz</v>
+        <v>Savinho</v>
       </c>
       <c r="B50" t="str">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C50" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D50" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/480692-1697903145.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/743591-1719653229.jpg?lm=1</v>
       </c>
       <c r="E50" t="str">
-        <v>Colombia</v>
+        <v>Brasil</v>
       </c>
       <c r="F50" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/83.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
       <c r="G50" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H50" t="str">
-        <v>Liverpool FC</v>
+        <v>Manchester City</v>
       </c>
       <c r="I50" t="str">
-        <v>70,00 mill. €</v>
-      </c>
-      <c r="L50" t="str">
-        <v>85,00 mill. €</v>
-      </c>
-      <c r="M50" t="str">
-        <v>30/05/2025</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J50" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K50" t="str">
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Cody Gakpo</v>
+        <v>Jarrad Branthwaite</v>
       </c>
       <c r="B51" t="str">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C51" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Defensa central</v>
       </c>
       <c r="D51" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/434675-1682690965.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/661053-1687975679.jpg?lm=1</v>
       </c>
       <c r="E51" t="str">
-        <v>Países Bajos</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F51" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G51" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/29.png?lm=1445949846</v>
       </c>
       <c r="H51" t="str">
-        <v>Liverpool FC</v>
+        <v>Everton FC</v>
       </c>
       <c r="I51" t="str">
-        <v>70,00 mill. €</v>
+        <v>50,00 mill. €</v>
       </c>
       <c r="J51" t="str">
-        <v>Togo</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K51" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/168.png?lm=1520611569</v>
-      </c>
-      <c r="L51" t="str">
-        <v>70,00 mill. €</v>
-      </c>
-      <c r="M51" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Kai Havertz</v>
+        <v>Kobbie Mainoo</v>
       </c>
       <c r="B52" t="str">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C52" t="str">
-        <v>Delantero centro</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D52" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/309400-1683903902.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/820374-1719349758.jpg?lm=1</v>
       </c>
       <c r="E52" t="str">
-        <v>Alemania</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F52" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/40.png?lm=1520612525</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G52" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H52" t="str">
-        <v>Arsenal FC</v>
+        <v>Manchester United</v>
       </c>
       <c r="I52" t="str">
-        <v>65,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J52" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K52" t="str">
+        <v>50,00 mill. €</v>
       </c>
       <c r="L52" t="str">
-        <v>90,00 mill. €</v>
+        <v>Ghana</v>
       </c>
       <c r="M52" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/54.png?lm=1520611569</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Anthony Gordon</v>
+        <v>Ben White</v>
       </c>
       <c r="B53" t="str">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C53" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Lateral derecho</v>
       </c>
       <c r="D53" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/503733-1660588736.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/335721-1683275943.jpg?lm=1</v>
       </c>
       <c r="E53" t="str">
         <v>Inglaterra</v>
@@ -2116,39 +2386,39 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G53" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H53" t="str">
-        <v>Newcastle United</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I53" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="L53" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="M53" t="str">
-        <v>30/05/2025</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J53" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K53" t="str">
+        <v>45,00 mill. €</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Rúben Dias</v>
+        <v>Rayan Cherki</v>
       </c>
       <c r="B54" t="str">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C54" t="str">
-        <v>Defensa central</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D54" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/258004-1684921271.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/607223-1672831487.jpg?lm=1</v>
       </c>
       <c r="E54" t="str">
-        <v>Portugal</v>
+        <v>Francia</v>
       </c>
       <c r="F54" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
       </c>
       <c r="G54" t="str">
         <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
@@ -2157,325 +2427,337 @@
         <v>Manchester City</v>
       </c>
       <c r="I54" t="str">
-        <v>65,00 mill. €</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J54" t="str">
+        <v>03/06/2025</v>
+      </c>
+      <c r="K54" t="str">
+        <v>45,00 mill. €</v>
       </c>
       <c r="L54" t="str">
-        <v>80,00 mill. €</v>
+        <v>Argelia</v>
       </c>
       <c r="M54" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/4.png?lm=1520611569</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Tijjani Reijnders</v>
+        <v>Myles Lewis-Skelly</v>
       </c>
       <c r="B55" t="str">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C55" t="str">
-        <v>Mediocentro</v>
+        <v>Lateral izquierdo</v>
       </c>
       <c r="D55" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/460939-1676466080.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/890721-1682599516.jpg?lm=1</v>
       </c>
       <c r="E55" t="str">
-        <v>Países Bajos</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F55" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G55" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H55" t="str">
-        <v>Manchester City</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I55" t="str">
-        <v>60,00 mill. €</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J55" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K55" t="str">
+        <v>45,00 mill. €</v>
       </c>
       <c r="L55" t="str">
-        <v>60,00 mill. €</v>
+        <v>Barbados</v>
       </c>
       <c r="M55" t="str">
-        <v>17/06/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/17.png?lm=1520611569</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>Matheus Cunha</v>
+        <v>Adam Wharton</v>
       </c>
       <c r="B56" t="str">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C56" t="str">
-        <v>Mediapunta</v>
+        <v>Pivote</v>
       </c>
       <c r="D56" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/517894-1696599737.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/744149-1716297290.jpg?lm=1</v>
       </c>
       <c r="E56" t="str">
-        <v>Brasil</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F56" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G56" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/543.png?lm=1467496784</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/873.png?lm=1457723287</v>
       </c>
       <c r="H56" t="str">
-        <v>Wolverhampton Wanderers</v>
+        <v>Crystal Palace</v>
       </c>
       <c r="I56" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="L56" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="M56" t="str">
-        <v>30/05/2025</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J56" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K56" t="str">
+        <v>45,00 mill. €</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>Erling Haaland</v>
+        <v>Marc Guéhi</v>
       </c>
       <c r="B57" t="str">
         <v>24</v>
       </c>
       <c r="C57" t="str">
-        <v>Delantero centro</v>
+        <v>Defensa central</v>
       </c>
       <c r="D57" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/418560-1709108116.png?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/392757-1683030598.jpg?lm=1</v>
       </c>
       <c r="E57" t="str">
-        <v>Noruega</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F57" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/125.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G57" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/873.png?lm=1457723287</v>
       </c>
       <c r="H57" t="str">
-        <v>Manchester City</v>
+        <v>Crystal Palace</v>
       </c>
       <c r="I57" t="str">
-        <v>180,00 mill. €</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J57" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K57" t="str">
+        <v>45,00 mill. €</v>
       </c>
       <c r="L57" t="str">
-        <v>200,00 mill. €</v>
+        <v>Costa de Marfil</v>
       </c>
       <c r="M57" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/38.png?lm=1520611569</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Bukayo Saka</v>
+        <v>Manuel Ugarte</v>
       </c>
       <c r="B58" t="str">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C58" t="str">
-        <v>Extremo derecho</v>
+        <v>Pivote</v>
       </c>
       <c r="D58" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/433177-1684155052.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/476701-1715107512.jpg?lm=1</v>
       </c>
       <c r="E58" t="str">
-        <v>Inglaterra</v>
+        <v>Uruguay</v>
       </c>
       <c r="F58" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/179.png?lm=1520611569</v>
       </c>
       <c r="G58" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H58" t="str">
-        <v>Arsenal FC</v>
+        <v>Manchester United</v>
       </c>
       <c r="I58" t="str">
-        <v>150,00 mill. €</v>
+        <v>60,00 mill. €</v>
       </c>
       <c r="J58" t="str">
-        <v>Nigeria</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K58" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
-      </c>
-      <c r="L58" t="str">
-        <v>150,00 mill. €</v>
-      </c>
-      <c r="M58" t="str">
-        <v>30/05/2025</v>
+        <v>45,00 mill. €</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Alexander Isak</v>
+        <v>Amad Diallo</v>
       </c>
       <c r="B59" t="str">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C59" t="str">
-        <v>Delantero centro</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D59" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/349066-1680791339.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/536835-1747857754.jpg?lm=1</v>
       </c>
       <c r="E59" t="str">
-        <v>Suecia</v>
+        <v>Costa de Marfil</v>
       </c>
       <c r="F59" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/38.png?lm=1520611569</v>
       </c>
       <c r="G59" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H59" t="str">
-        <v>Newcastle United</v>
+        <v>Manchester United</v>
       </c>
       <c r="I59" t="str">
-        <v>120,00 mill. €</v>
+        <v>45,00 mill. €</v>
       </c>
       <c r="J59" t="str">
-        <v>Eritrea</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K59" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/46.png?lm=1520611569</v>
+        <v>45,00 mill. €</v>
       </c>
       <c r="L59" t="str">
-        <v>120,00 mill. €</v>
+        <v>Italia</v>
       </c>
       <c r="M59" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Declan Rice</v>
+        <v>Darwin Núñez</v>
       </c>
       <c r="B60" t="str">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" t="str">
-        <v>Mediocentro</v>
+        <v>Delantero centro</v>
       </c>
       <c r="D60" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/357662-1687962936.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/546543-1681827179.jpg?lm=1</v>
       </c>
       <c r="E60" t="str">
-        <v>Inglaterra</v>
+        <v>Uruguay</v>
       </c>
       <c r="F60" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/179.png?lm=1520611569</v>
       </c>
       <c r="G60" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
       </c>
       <c r="H60" t="str">
-        <v>Arsenal FC</v>
+        <v>Liverpool FC</v>
       </c>
       <c r="I60" t="str">
-        <v>120,00 mill. €</v>
+        <v>70,00 mill. €</v>
       </c>
       <c r="J60" t="str">
-        <v>Irlanda</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K60" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/72.png?lm=1520611569</v>
-      </c>
-      <c r="L60" t="str">
-        <v>120,00 mill. €</v>
-      </c>
-      <c r="M60" t="str">
-        <v>30/05/2025</v>
+        <v>45,00 mill. €</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Cole Palmer</v>
+        <v>Mohammed Kudus</v>
       </c>
       <c r="B61" t="str">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C61" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D61" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/568177-1712320986.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/543499-1668429218.jpg?lm=1</v>
       </c>
       <c r="E61" t="str">
-        <v>Inglaterra</v>
+        <v>Ghana</v>
       </c>
       <c r="F61" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/54.png?lm=1520611569</v>
       </c>
       <c r="G61" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/379.png?lm=1464675260</v>
       </c>
       <c r="H61" t="str">
-        <v>Chelsea FC</v>
+        <v>West Ham United</v>
       </c>
       <c r="I61" t="str">
-        <v>120,00 mill. €</v>
-      </c>
-      <c r="L61" t="str">
-        <v>130,00 mill. €</v>
-      </c>
-      <c r="M61" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
+      </c>
+      <c r="J61" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K61" t="str">
+        <v>45,00 mill. €</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>Rodri</v>
+        <v>Milos Kerkez</v>
       </c>
       <c r="B62" t="str">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C62" t="str">
-        <v>Pivote</v>
+        <v>Lateral izquierdo</v>
       </c>
       <c r="D62" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/357565-1682587890.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/730861-1660762995.jpg?lm=1</v>
       </c>
       <c r="E62" t="str">
-        <v>España</v>
+        <v>Hungría</v>
       </c>
       <c r="F62" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/178.png?lm=1521635893</v>
       </c>
       <c r="G62" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/989.png?lm=1457991811</v>
       </c>
       <c r="H62" t="str">
-        <v>Manchester City</v>
+        <v>AFC Bournemouth</v>
       </c>
       <c r="I62" t="str">
-        <v>110,00 mill. €</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J62" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K62" t="str">
+        <v>45,00 mill. €</v>
       </c>
       <c r="L62" t="str">
-        <v>130,00 mill. €</v>
+        <v>Serbia</v>
       </c>
       <c r="M62" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/215.png?lm=1520611569</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Phil Foden</v>
+        <v>Curtis Jones</v>
       </c>
       <c r="B63" t="str">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C63" t="str">
-        <v>Extremo derecho</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D63" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/406635-1668524492.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/433188-1701681163.jpg?lm=1</v>
       </c>
       <c r="E63" t="str">
         <v>Inglaterra</v>
@@ -2484,33 +2766,33 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G63" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
       </c>
       <c r="H63" t="str">
-        <v>Manchester City</v>
+        <v>Liverpool FC</v>
       </c>
       <c r="I63" t="str">
-        <v>100,00 mill. €</v>
-      </c>
-      <c r="L63" t="str">
-        <v>150,00 mill. €</v>
-      </c>
-      <c r="M63" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
+      </c>
+      <c r="J63" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K63" t="str">
+        <v>45,00 mill. €</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>Alexis Mac Allister</v>
+        <v>Alejandro Garnacho</v>
       </c>
       <c r="B64" t="str">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C64" t="str">
-        <v>Mediocentro</v>
+        <v>Mediocentro ofensivo</v>
       </c>
       <c r="D64" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/534033-1669835342.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/811779-1703629085.jpg?lm=1</v>
       </c>
       <c r="E64" t="str">
         <v>Argentina</v>
@@ -2519,495 +2801,495 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
       </c>
       <c r="G64" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H64" t="str">
-        <v>Liverpool FC</v>
+        <v>Manchester United</v>
       </c>
       <c r="I64" t="str">
-        <v>100,00 mill. €</v>
+        <v>50,00 mill. €</v>
       </c>
       <c r="J64" t="str">
-        <v>Italia</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K64" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
+        <v>45,00 mill. €</v>
       </c>
       <c r="L64" t="str">
-        <v>100,00 mill. €</v>
+        <v>España</v>
       </c>
       <c r="M64" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Moisés Caicedo</v>
+        <v>Anthony Elanga</v>
       </c>
       <c r="B65" t="str">
         <v>23</v>
       </c>
       <c r="C65" t="str">
-        <v>Pivote</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D65" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/687626-1660729724.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/583189-1700739021.jpg?lm=1</v>
       </c>
       <c r="E65" t="str">
-        <v>Ecuador</v>
+        <v>Suecia</v>
       </c>
       <c r="F65" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/44.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
       </c>
       <c r="G65" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/703.png?lm=1598890289</v>
       </c>
       <c r="H65" t="str">
-        <v>Chelsea FC</v>
+        <v>Nottingham Forest</v>
       </c>
       <c r="I65" t="str">
-        <v>90,00 mill. €</v>
+        <v>42,00 mill. €</v>
+      </c>
+      <c r="J65" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K65" t="str">
+        <v>42,00 mill. €</v>
       </c>
       <c r="L65" t="str">
-        <v>90,00 mill. €</v>
+        <v>Camerún</v>
       </c>
       <c r="M65" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Martin Ødegaard</v>
+        <v>Sven Botman</v>
       </c>
       <c r="B66" t="str">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C66" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Defensa central</v>
       </c>
       <c r="D66" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/316264-1678877651.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/361093-1683290679.jpg?lm=1</v>
       </c>
       <c r="E66" t="str">
-        <v>Noruega</v>
+        <v>Países Bajos</v>
       </c>
       <c r="F66" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/125.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
       </c>
       <c r="G66" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
       </c>
       <c r="H66" t="str">
-        <v>Arsenal FC</v>
+        <v>Newcastle United</v>
       </c>
       <c r="I66" t="str">
-        <v>85,00 mill. €</v>
-      </c>
-      <c r="L66" t="str">
-        <v>110,00 mill. €</v>
-      </c>
-      <c r="M66" t="str">
-        <v>30/05/2025</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J66" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K66" t="str">
+        <v>42,00 mill. €</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>William Saliba</v>
+        <v>James Maddison</v>
       </c>
       <c r="B67" t="str">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C67" t="str">
-        <v>Defensa central</v>
+        <v>Mediocentro ofensivo</v>
       </c>
       <c r="D67" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/495666-1718697201.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/294057-1687982662.jpg?lm=1</v>
       </c>
       <c r="E67" t="str">
-        <v>Francia</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F67" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G67" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H67" t="str">
-        <v>Arsenal FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I67" t="str">
-        <v>80,00 mill. €</v>
+        <v>70,00 mill. €</v>
       </c>
       <c r="J67" t="str">
-        <v>Camerún</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K67" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
-      </c>
-      <c r="L67" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="M67" t="str">
-        <v>30/05/2025</v>
+        <v>42,00 mill. €</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Bruno Guimarães</v>
+        <v>Ilya Zabarnyi</v>
       </c>
       <c r="B68" t="str">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C68" t="str">
-        <v>Pivote</v>
+        <v>Defensa central</v>
       </c>
       <c r="D68" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/520624-1668522672.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/659089-1715881375.jpg?lm=1</v>
       </c>
       <c r="E68" t="str">
-        <v>Brasil</v>
+        <v>Ucrania</v>
       </c>
       <c r="F68" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/177.png?lm=1520611569</v>
       </c>
       <c r="G68" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/989.png?lm=1457991811</v>
       </c>
       <c r="H68" t="str">
-        <v>Newcastle United</v>
+        <v>AFC Bournemouth</v>
       </c>
       <c r="I68" t="str">
-        <v>80,00 mill. €</v>
+        <v>42,00 mill. €</v>
       </c>
       <c r="J68" t="str">
-        <v>España</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K68" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
-      </c>
-      <c r="L68" t="str">
-        <v>85,00 mill. €</v>
-      </c>
-      <c r="M68" t="str">
-        <v>30/05/2025</v>
+        <v>42,00 mill. €</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>Dominik Szoboszlai</v>
+        <v>Antoine Semenyo</v>
       </c>
       <c r="B69" t="str">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C69" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Extremo izquierdo</v>
       </c>
       <c r="D69" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/451276-1700209677.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/583255-1737452028.jpg?lm=1</v>
       </c>
       <c r="E69" t="str">
-        <v>Hungría</v>
+        <v>Ghana</v>
       </c>
       <c r="F69" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/178.png?lm=1521635893</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/54.png?lm=1520611569</v>
       </c>
       <c r="G69" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/989.png?lm=1457991811</v>
       </c>
       <c r="H69" t="str">
-        <v>Liverpool FC</v>
+        <v>AFC Bournemouth</v>
       </c>
       <c r="I69" t="str">
-        <v>80,00 mill. €</v>
+        <v>40,00 mill. €</v>
+      </c>
+      <c r="J69" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K69" t="str">
+        <v>40,00 mill. €</v>
       </c>
       <c r="L69" t="str">
-        <v>80,00 mill. €</v>
+        <v>Inglaterra</v>
       </c>
       <c r="M69" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Gabriel Magalhães</v>
+        <v>Carlos Baleba</v>
       </c>
       <c r="B70" t="str">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C70" t="str">
-        <v>Defensa central</v>
+        <v>Pivote</v>
       </c>
       <c r="D70" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/435338-1684162833.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/973085-1666690662.jpg?lm=1</v>
       </c>
       <c r="E70" t="str">
-        <v>Brasil</v>
+        <v>Camerún</v>
       </c>
       <c r="F70" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
       </c>
       <c r="G70" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/1237.png?lm=1492718902</v>
       </c>
       <c r="H70" t="str">
-        <v>Arsenal FC</v>
+        <v>Brighton &amp; Hove Albion</v>
       </c>
       <c r="I70" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="L70" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="M70" t="str">
-        <v>30/05/2025</v>
+        <v>40,00 mill. €</v>
+      </c>
+      <c r="J70" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K70" t="str">
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>Omar Marmoush</v>
+        <v>Brennan Johnson</v>
       </c>
       <c r="B71" t="str">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C71" t="str">
-        <v>Delantero centro</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D71" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/445939-1747656490.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/470607-1692959021.jpg?lm=1</v>
       </c>
       <c r="E71" t="str">
-        <v>Egipto</v>
+        <v>Gales</v>
       </c>
       <c r="F71" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/2.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/191.png?lm=1520611569</v>
       </c>
       <c r="G71" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H71" t="str">
-        <v>Manchester City</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I71" t="str">
-        <v>75,00 mill. €</v>
+        <v>50,00 mill. €</v>
       </c>
       <c r="J71" t="str">
-        <v>Canadá</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K71" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/80.png?lm=1520611569</v>
+        <v>40,00 mill. €</v>
       </c>
       <c r="L71" t="str">
-        <v>75,00 mill. €</v>
+        <v>Inglaterra</v>
       </c>
       <c r="M71" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Josko Gvardiol</v>
+        <v>Kaoru Mitoma</v>
       </c>
       <c r="B72" t="str">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C72" t="str">
-        <v>Lateral izquierdo</v>
+        <v>Extremo izquierdo</v>
       </c>
       <c r="D72" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/475959-1713391602.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/504849-1731683095.jpg?lm=1</v>
       </c>
       <c r="E72" t="str">
-        <v>Croacia</v>
+        <v>Japón</v>
       </c>
       <c r="F72" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/37.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/77.png?lm=1520611569</v>
       </c>
       <c r="G72" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/1237.png?lm=1492718902</v>
       </c>
       <c r="H72" t="str">
-        <v>Manchester City</v>
+        <v>Brighton &amp; Hove Albion</v>
       </c>
       <c r="I72" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="L72" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="M72" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
+      </c>
+      <c r="J72" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K72" t="str">
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Enzo Fernández</v>
+        <v>Destiny Udogie</v>
       </c>
       <c r="B73" t="str">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C73" t="str">
-        <v>Mediocentro</v>
+        <v>Lateral izquierdo</v>
       </c>
       <c r="D73" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/648195-1669894717.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/556385-1697208468.jpg?lm=1</v>
       </c>
       <c r="E73" t="str">
-        <v>Argentina</v>
+        <v>Italia</v>
       </c>
       <c r="F73" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
       </c>
       <c r="G73" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H73" t="str">
-        <v>Chelsea FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I73" t="str">
-        <v>75,00 mill. €</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J73" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K73" t="str">
+        <v>40,00 mill. €</v>
       </c>
       <c r="L73" t="str">
-        <v>85,00 mill. €</v>
+        <v>Nigeria</v>
       </c>
       <c r="M73" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>Ryan Gravenberch</v>
+        <v>Lisandro Martínez</v>
       </c>
       <c r="B74" t="str">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C74" t="str">
-        <v>Pivote</v>
+        <v>Defensa central</v>
       </c>
       <c r="D74" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/478573-1718097194.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/480762-1680681507.jpg?lm=1</v>
       </c>
       <c r="E74" t="str">
-        <v>Países Bajos</v>
+        <v>Argentina</v>
       </c>
       <c r="F74" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
       </c>
       <c r="G74" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H74" t="str">
-        <v>Liverpool FC</v>
+        <v>Manchester United</v>
       </c>
       <c r="I74" t="str">
-        <v>75,00 mill. €</v>
+        <v>50,00 mill. €</v>
       </c>
       <c r="J74" t="str">
-        <v>Surinam</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K74" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/161.png?lm=1520611569</v>
-      </c>
-      <c r="L74" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="M74" t="str">
-        <v>30/05/2025</v>
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Cody Gakpo</v>
+        <v>Noni Madueke</v>
       </c>
       <c r="B75" t="str">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C75" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D75" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/434675-1682690965.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/503987-1683102348.jpg?lm=1</v>
       </c>
       <c r="E75" t="str">
-        <v>Países Bajos</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F75" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G75" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H75" t="str">
-        <v>Liverpool FC</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I75" t="str">
-        <v>70,00 mill. €</v>
+        <v>40,00 mill. €</v>
       </c>
       <c r="J75" t="str">
-        <v>Togo</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K75" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/168.png?lm=1520611569</v>
+        <v>40,00 mill. €</v>
       </c>
       <c r="L75" t="str">
-        <v>70,00 mill. €</v>
+        <v>Nigeria</v>
       </c>
       <c r="M75" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>Luis Díaz</v>
+        <v>Jarrod Bowen</v>
       </c>
       <c r="B76" t="str">
         <v>28</v>
       </c>
       <c r="C76" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Extremo derecho</v>
       </c>
       <c r="D76" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/480692-1697903145.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/314875-1662362005.jpg?lm=1</v>
       </c>
       <c r="E76" t="str">
-        <v>Colombia</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F76" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/83.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G76" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/379.png?lm=1464675260</v>
       </c>
       <c r="H76" t="str">
-        <v>Liverpool FC</v>
+        <v>West Ham United</v>
       </c>
       <c r="I76" t="str">
-        <v>70,00 mill. €</v>
-      </c>
-      <c r="L76" t="str">
-        <v>85,00 mill. €</v>
-      </c>
-      <c r="M76" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
+      </c>
+      <c r="J76" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K76" t="str">
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>Rúben Dias</v>
+        <v>Nico González</v>
       </c>
       <c r="B77" t="str">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C77" t="str">
-        <v>Defensa central</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D77" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/258004-1684921271.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/466805-1743669968.jpg?lm=1</v>
       </c>
       <c r="E77" t="str">
-        <v>Portugal</v>
+        <v>España</v>
       </c>
       <c r="F77" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
       </c>
       <c r="G77" t="str">
         <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
@@ -3016,62 +3298,62 @@
         <v>Manchester City</v>
       </c>
       <c r="I77" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="L77" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="M77" t="str">
-        <v>30/05/2025</v>
+        <v>40,00 mill. €</v>
+      </c>
+      <c r="J77" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K77" t="str">
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>Kai Havertz</v>
+        <v>Diogo Jota</v>
       </c>
       <c r="B78" t="str">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C78" t="str">
         <v>Delantero centro</v>
       </c>
       <c r="D78" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/309400-1683903902.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/340950-1716296423.jpg?lm=1</v>
       </c>
       <c r="E78" t="str">
-        <v>Alemania</v>
+        <v>Portugal</v>
       </c>
       <c r="F78" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/40.png?lm=1520612525</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
       </c>
       <c r="G78" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
       </c>
       <c r="H78" t="str">
-        <v>Arsenal FC</v>
+        <v>Liverpool FC</v>
       </c>
       <c r="I78" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="L78" t="str">
-        <v>90,00 mill. €</v>
-      </c>
-      <c r="M78" t="str">
-        <v>30/05/2025</v>
+        <v>60,00 mill. €</v>
+      </c>
+      <c r="J78" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K78" t="str">
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>Anthony Gordon</v>
+        <v>Liam Delap</v>
       </c>
       <c r="B79" t="str">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C79" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Delantero centro</v>
       </c>
       <c r="D79" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/503733-1660588736.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/610849-1746646306.jpg?lm=1</v>
       </c>
       <c r="E79" t="str">
         <v>Inglaterra</v>
@@ -3080,138 +3362,150 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G79" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H79" t="str">
-        <v>Newcastle United</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I79" t="str">
-        <v>65,00 mill. €</v>
+        <v>40,00 mill. €</v>
+      </c>
+      <c r="J79" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K79" t="str">
+        <v>40,00 mill. €</v>
       </c>
       <c r="L79" t="str">
-        <v>65,00 mill. €</v>
+        <v>Irlanda</v>
       </c>
       <c r="M79" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/72.png?lm=1520611569</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>Sandro Tonali</v>
+        <v>David Raya</v>
       </c>
       <c r="B80" t="str">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C80" t="str">
-        <v>Mediocentro</v>
+        <v>Portero</v>
       </c>
       <c r="D80" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/397033-1688389270.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/262749-1668168018.jpg?lm=1</v>
       </c>
       <c r="E80" t="str">
-        <v>Italia</v>
+        <v>España</v>
       </c>
       <c r="F80" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
       </c>
       <c r="G80" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H80" t="str">
-        <v>Newcastle United</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I80" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="L80" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="M80" t="str">
-        <v>30/05/2025</v>
+        <v>40,00 mill. €</v>
+      </c>
+      <c r="J80" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K80" t="str">
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>Tijjani Reijnders</v>
+        <v>Dominic Solanke</v>
       </c>
       <c r="B81" t="str">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C81" t="str">
-        <v>Mediocentro</v>
+        <v>Delantero centro</v>
       </c>
       <c r="D81" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/460939-1676466080.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/258889-1708340487.jpg?lm=1</v>
       </c>
       <c r="E81" t="str">
-        <v>Países Bajos</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F81" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G81" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H81" t="str">
-        <v>Manchester City</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I81" t="str">
-        <v>60,00 mill. €</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J81" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K81" t="str">
+        <v>40,00 mill. €</v>
       </c>
       <c r="L81" t="str">
-        <v>60,00 mill. €</v>
+        <v>Nigeria</v>
       </c>
       <c r="M81" t="str">
-        <v>17/06/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>Erling Haaland</v>
+        <v>Ollie Watkins</v>
       </c>
       <c r="B82" t="str">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C82" t="str">
         <v>Delantero centro</v>
       </c>
       <c r="D82" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/418560-1709108116.png?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/324358-1708341279.jpg?lm=1</v>
       </c>
       <c r="E82" t="str">
-        <v>Noruega</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F82" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/125.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G82" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/405.png?lm=1717155982</v>
       </c>
       <c r="H82" t="str">
-        <v>Manchester City</v>
+        <v>Aston Villa</v>
       </c>
       <c r="I82" t="str">
-        <v>180,00 mill. €</v>
-      </c>
-      <c r="L82" t="str">
-        <v>200,00 mill. €</v>
-      </c>
-      <c r="M82" t="str">
-        <v>30/05/2025</v>
+        <v>65,00 mill. €</v>
+      </c>
+      <c r="J82" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K82" t="str">
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>Bukayo Saka</v>
+        <v>Rico Lewis</v>
       </c>
       <c r="B83" t="str">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C83" t="str">
-        <v>Extremo derecho</v>
+        <v>Lateral derecho</v>
       </c>
       <c r="D83" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/433177-1684155052.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/701057-1684856684.jpg?lm=1</v>
       </c>
       <c r="E83" t="str">
         <v>Inglaterra</v>
@@ -3220,571 +3514,565 @@
         <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G83" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H83" t="str">
-        <v>Arsenal FC</v>
+        <v>Manchester City</v>
       </c>
       <c r="I83" t="str">
-        <v>150,00 mill. €</v>
+        <v>40,00 mill. €</v>
       </c>
       <c r="J83" t="str">
-        <v>Nigeria</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K83" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/124.png?lm=1520611569</v>
-      </c>
-      <c r="L83" t="str">
-        <v>150,00 mill. €</v>
-      </c>
-      <c r="M83" t="str">
-        <v>30/05/2025</v>
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>Alexander Isak</v>
+        <v>Roméo Lavia</v>
       </c>
       <c r="B84" t="str">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C84" t="str">
-        <v>Delantero centro</v>
+        <v>Pivote</v>
       </c>
       <c r="D84" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/349066-1680791339.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/628451-1683898478.jpg?lm=1</v>
       </c>
       <c r="E84" t="str">
-        <v>Suecia</v>
+        <v>Bélgica</v>
       </c>
       <c r="F84" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/19.png?lm=1520611569</v>
       </c>
       <c r="G84" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H84" t="str">
-        <v>Newcastle United</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I84" t="str">
-        <v>120,00 mill. €</v>
+        <v>50,00 mill. €</v>
       </c>
       <c r="J84" t="str">
-        <v>Eritrea</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K84" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/46.png?lm=1520611569</v>
-      </c>
-      <c r="L84" t="str">
-        <v>120,00 mill. €</v>
-      </c>
-      <c r="M84" t="str">
-        <v>30/05/2025</v>
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>Declan Rice</v>
+        <v>João Gomes</v>
       </c>
       <c r="B85" t="str">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C85" t="str">
         <v>Mediocentro</v>
       </c>
       <c r="D85" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/357662-1687962936.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/735570-1675092223.jpg?lm=1</v>
       </c>
       <c r="E85" t="str">
-        <v>Inglaterra</v>
+        <v>Brasil</v>
       </c>
       <c r="F85" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
       <c r="G85" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/543.png?lm=1467496784</v>
       </c>
       <c r="H85" t="str">
-        <v>Arsenal FC</v>
+        <v>Wolverhampton Wanderers</v>
       </c>
       <c r="I85" t="str">
-        <v>120,00 mill. €</v>
+        <v>40,00 mill. €</v>
       </c>
       <c r="J85" t="str">
-        <v>Irlanda</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K85" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/72.png?lm=1520611569</v>
-      </c>
-      <c r="L85" t="str">
-        <v>120,00 mill. €</v>
-      </c>
-      <c r="M85" t="str">
-        <v>30/05/2025</v>
+        <v>40,00 mill. €</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>Cole Palmer</v>
+        <v>Boubacar Kamara</v>
       </c>
       <c r="B86" t="str">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C86" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Pivote</v>
       </c>
       <c r="D86" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/568177-1712320986.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/394327-1736160460.jpg?lm=1</v>
       </c>
       <c r="E86" t="str">
-        <v>Inglaterra</v>
+        <v>Francia</v>
       </c>
       <c r="F86" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
       </c>
       <c r="G86" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/405.png?lm=1717155982</v>
       </c>
       <c r="H86" t="str">
-        <v>Chelsea FC</v>
+        <v>Aston Villa</v>
       </c>
       <c r="I86" t="str">
-        <v>120,00 mill. €</v>
+        <v>40,00 mill. €</v>
+      </c>
+      <c r="J86" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K86" t="str">
+        <v>40,00 mill. €</v>
       </c>
       <c r="L86" t="str">
-        <v>130,00 mill. €</v>
+        <v>Senegal</v>
       </c>
       <c r="M86" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/149.png?lm=1520611569</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>Rodri</v>
+        <v>Tino Livramento</v>
       </c>
       <c r="B87" t="str">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C87" t="str">
-        <v>Pivote</v>
+        <v>Lateral derecho</v>
       </c>
       <c r="D87" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/357565-1682587890.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/503981-1699383321.jpg?lm=1</v>
       </c>
       <c r="E87" t="str">
-        <v>España</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F87" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G87" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
       </c>
       <c r="H87" t="str">
-        <v>Manchester City</v>
+        <v>Newcastle United</v>
       </c>
       <c r="I87" t="str">
-        <v>110,00 mill. €</v>
+        <v>40,00 mill. €</v>
+      </c>
+      <c r="J87" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K87" t="str">
+        <v>40,00 mill. €</v>
       </c>
       <c r="L87" t="str">
-        <v>130,00 mill. €</v>
+        <v>Escocia</v>
       </c>
       <c r="M87" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/190.png?lm=1520611569</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>Phil Foden</v>
+        <v>Youri Tielemans</v>
       </c>
       <c r="B88" t="str">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C88" t="str">
-        <v>Extremo derecho</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D88" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/406635-1668524492.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/249565-1716886438.jpg?lm=1</v>
       </c>
       <c r="E88" t="str">
-        <v>Inglaterra</v>
+        <v>Bélgica</v>
       </c>
       <c r="F88" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/19.png?lm=1520611569</v>
       </c>
       <c r="G88" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/405.png?lm=1717155982</v>
       </c>
       <c r="H88" t="str">
-        <v>Manchester City</v>
+        <v>Aston Villa</v>
       </c>
       <c r="I88" t="str">
-        <v>100,00 mill. €</v>
+        <v>55,00 mill. €</v>
+      </c>
+      <c r="J88" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K88" t="str">
+        <v>38,00 mill. €</v>
       </c>
       <c r="L88" t="str">
-        <v>150,00 mill. €</v>
+        <v>RD del Congo</v>
       </c>
       <c r="M88" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/193.png?lm=1520611569</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>Alexis Mac Allister</v>
+        <v>Lucas Bergvall</v>
       </c>
       <c r="B89" t="str">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C89" t="str">
         <v>Mediocentro</v>
       </c>
       <c r="D89" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/534033-1669835342.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/866246-1701861399.jpg?lm=1</v>
       </c>
       <c r="E89" t="str">
-        <v>Argentina</v>
+        <v>Suecia</v>
       </c>
       <c r="F89" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/147.png?lm=1520611569</v>
       </c>
       <c r="G89" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H89" t="str">
-        <v>Liverpool FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I89" t="str">
-        <v>100,00 mill. €</v>
+        <v>38,00 mill. €</v>
       </c>
       <c r="J89" t="str">
-        <v>Italia</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K89" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
-      </c>
-      <c r="L89" t="str">
-        <v>100,00 mill. €</v>
-      </c>
-      <c r="M89" t="str">
-        <v>30/05/2025</v>
+        <v>38,00 mill. €</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>Moisés Caicedo</v>
+        <v>Pedro Porro</v>
       </c>
       <c r="B90" t="str">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C90" t="str">
-        <v>Pivote</v>
+        <v>Lateral derecho</v>
       </c>
       <c r="D90" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/687626-1660729724.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/553875-1730812390.jpg?lm=1</v>
       </c>
       <c r="E90" t="str">
-        <v>Ecuador</v>
+        <v>España</v>
       </c>
       <c r="F90" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/44.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
       </c>
       <c r="G90" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H90" t="str">
-        <v>Chelsea FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I90" t="str">
-        <v>90,00 mill. €</v>
-      </c>
-      <c r="L90" t="str">
-        <v>90,00 mill. €</v>
-      </c>
-      <c r="M90" t="str">
-        <v>30/05/2025</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J90" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K90" t="str">
+        <v>38,00 mill. €</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>Martin Ødegaard</v>
+        <v>Archie Gray</v>
       </c>
       <c r="B91" t="str">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C91" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Pivote</v>
       </c>
       <c r="D91" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/316264-1678877651.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/922693-1695108880.jpg?lm=1</v>
       </c>
       <c r="E91" t="str">
-        <v>Noruega</v>
+        <v>Inglaterra</v>
       </c>
       <c r="F91" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/125.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
       <c r="G91" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/148.png?lm=1732011953</v>
       </c>
       <c r="H91" t="str">
-        <v>Arsenal FC</v>
+        <v>Tottenham Hotspur</v>
       </c>
       <c r="I91" t="str">
-        <v>85,00 mill. €</v>
+        <v>38,00 mill. €</v>
+      </c>
+      <c r="J91" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K91" t="str">
+        <v>38,00 mill. €</v>
       </c>
       <c r="L91" t="str">
-        <v>110,00 mill. €</v>
+        <v>Escocia</v>
       </c>
       <c r="M91" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/190.png?lm=1520611569</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>William Saliba</v>
+        <v>Bernardo Silva</v>
       </c>
       <c r="B92" t="str">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C92" t="str">
-        <v>Defensa central</v>
+        <v>Mediocentro ofensivo</v>
       </c>
       <c r="D92" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/495666-1718697201.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/241641-1684311533.jpg?lm=1</v>
       </c>
       <c r="E92" t="str">
-        <v>Francia</v>
+        <v>Portugal</v>
       </c>
       <c r="F92" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
       </c>
       <c r="G92" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H92" t="str">
-        <v>Arsenal FC</v>
+        <v>Manchester City</v>
       </c>
       <c r="I92" t="str">
-        <v>80,00 mill. €</v>
+        <v>100,00 mill. €</v>
       </c>
       <c r="J92" t="str">
-        <v>Camerún</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K92" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/31.png?lm=1520611569</v>
-      </c>
-      <c r="L92" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="M92" t="str">
-        <v>30/05/2025</v>
+        <v>38,00 mill. €</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>Bruno Guimarães</v>
+        <v>Matthijs de Ligt</v>
       </c>
       <c r="B93" t="str">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C93" t="str">
-        <v>Pivote</v>
+        <v>Defensa central</v>
       </c>
       <c r="D93" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/520624-1668522672.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/326031-1700659567.jpg?lm=1</v>
       </c>
       <c r="E93" t="str">
-        <v>Brasil</v>
+        <v>Países Bajos</v>
       </c>
       <c r="F93" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
       </c>
       <c r="G93" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H93" t="str">
-        <v>Newcastle United</v>
+        <v>Manchester United</v>
       </c>
       <c r="I93" t="str">
-        <v>80,00 mill. €</v>
+        <v>75,00 mill. €</v>
       </c>
       <c r="J93" t="str">
-        <v>España</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K93" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
-      </c>
-      <c r="L93" t="str">
-        <v>85,00 mill. €</v>
-      </c>
-      <c r="M93" t="str">
-        <v>30/05/2025</v>
+        <v>38,00 mill. €</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>Dominik Szoboszlai</v>
+        <v>Mikel Merino</v>
       </c>
       <c r="B94" t="str">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C94" t="str">
-        <v>Mediocentro ofensivo</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D94" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/451276-1700209677.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/338424-1716803831.jpg?lm=1</v>
       </c>
       <c r="E94" t="str">
-        <v>Hungría</v>
+        <v>España</v>
       </c>
       <c r="F94" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/178.png?lm=1521635893</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
       </c>
       <c r="G94" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H94" t="str">
-        <v>Liverpool FC</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I94" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="L94" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="M94" t="str">
-        <v>30/05/2025</v>
+        <v>50,00 mill. €</v>
+      </c>
+      <c r="J94" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K94" t="str">
+        <v>35,00 mill. €</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>Gabriel Magalhães</v>
+        <v>Rayan Aït-Nouri</v>
       </c>
       <c r="B95" t="str">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C95" t="str">
-        <v>Defensa central</v>
+        <v>Lateral izquierdo</v>
       </c>
       <c r="D95" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/435338-1684162833.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/578391-1695656762.jpg?lm=1</v>
       </c>
       <c r="E95" t="str">
-        <v>Brasil</v>
+        <v>Argelia</v>
       </c>
       <c r="F95" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/4.png?lm=1520611569</v>
       </c>
       <c r="G95" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H95" t="str">
-        <v>Arsenal FC</v>
+        <v>Manchester City</v>
       </c>
       <c r="I95" t="str">
-        <v>75,00 mill. €</v>
+        <v>35,00 mill. €</v>
+      </c>
+      <c r="J95" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K95" t="str">
+        <v>35,00 mill. €</v>
       </c>
       <c r="L95" t="str">
-        <v>75,00 mill. €</v>
+        <v>Francia</v>
       </c>
       <c r="M95" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>Omar Marmoush</v>
+        <v>Rasmus Højlund</v>
       </c>
       <c r="B96" t="str">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C96" t="str">
         <v>Delantero centro</v>
       </c>
       <c r="D96" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/445939-1747656490.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/610442-1699471458.jpg?lm=1</v>
       </c>
       <c r="E96" t="str">
-        <v>Egipto</v>
+        <v>Dinamarca</v>
       </c>
       <c r="F96" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/2.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/39.png?lm=1520611569</v>
       </c>
       <c r="G96" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/985.png?lm=1457975903</v>
       </c>
       <c r="H96" t="str">
-        <v>Manchester City</v>
+        <v>Manchester United</v>
       </c>
       <c r="I96" t="str">
-        <v>75,00 mill. €</v>
+        <v>65,00 mill. €</v>
       </c>
       <c r="J96" t="str">
-        <v>Canadá</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K96" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/80.png?lm=1520611569</v>
-      </c>
-      <c r="L96" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="M96" t="str">
-        <v>30/05/2025</v>
+        <v>35,00 mill. €</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>Josko Gvardiol</v>
+        <v>Antonee Robinson</v>
       </c>
       <c r="B97" t="str">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C97" t="str">
         <v>Lateral izquierdo</v>
       </c>
       <c r="D97" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/475959-1713391602.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/349701-1703926612.jpg?lm=1</v>
       </c>
       <c r="E97" t="str">
-        <v>Croacia</v>
+        <v>Estados Unidos</v>
       </c>
       <c r="F97" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/37.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/184.png?lm=1520611569</v>
       </c>
       <c r="G97" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/931.png?lm=1556831687</v>
       </c>
       <c r="H97" t="str">
-        <v>Manchester City</v>
+        <v>Fulham FC</v>
       </c>
       <c r="I97" t="str">
-        <v>75,00 mill. €</v>
+        <v>35,00 mill. €</v>
+      </c>
+      <c r="J97" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K97" t="str">
+        <v>35,00 mill. €</v>
       </c>
       <c r="L97" t="str">
-        <v>80,00 mill. €</v>
+        <v>Inglaterra</v>
       </c>
       <c r="M97" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>Enzo Fernández</v>
+        <v>Christopher Nkunku</v>
       </c>
       <c r="B98" t="str">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C98" t="str">
-        <v>Mediocentro</v>
+        <v>Mediocentro ofensivo</v>
       </c>
       <c r="D98" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/648195-1669894717.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/344381-1663686834.jpg?lm=1</v>
       </c>
       <c r="E98" t="str">
-        <v>Argentina</v>
+        <v>Francia</v>
       </c>
       <c r="F98" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/9.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/50.png?lm=1520611569</v>
       </c>
       <c r="G98" t="str">
         <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
@@ -3793,310 +4081,135 @@
         <v>Chelsea FC</v>
       </c>
       <c r="I98" t="str">
-        <v>75,00 mill. €</v>
+        <v>80,00 mill. €</v>
+      </c>
+      <c r="J98" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K98" t="str">
+        <v>35,00 mill. €</v>
       </c>
       <c r="L98" t="str">
-        <v>85,00 mill. €</v>
+        <v>RD del Congo</v>
       </c>
       <c r="M98" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/193.png?lm=1520611569</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>Ryan Gravenberch</v>
+        <v>Marc Cucurella</v>
       </c>
       <c r="B99" t="str">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C99" t="str">
-        <v>Pivote</v>
+        <v>Lateral izquierdo</v>
       </c>
       <c r="D99" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/478573-1718097194.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/284857-1659559729.jpg?lm=1</v>
       </c>
       <c r="E99" t="str">
-        <v>Países Bajos</v>
+        <v>España</v>
       </c>
       <c r="F99" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/157.png?lm=1520611569</v>
       </c>
       <c r="G99" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/631.png?lm=1682435911</v>
       </c>
       <c r="H99" t="str">
-        <v>Liverpool FC</v>
+        <v>Chelsea FC</v>
       </c>
       <c r="I99" t="str">
-        <v>75,00 mill. €</v>
+        <v>55,00 mill. €</v>
       </c>
       <c r="J99" t="str">
-        <v>Surinam</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K99" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/161.png?lm=1520611569</v>
-      </c>
-      <c r="L99" t="str">
-        <v>75,00 mill. €</v>
-      </c>
-      <c r="M99" t="str">
-        <v>30/05/2025</v>
+        <v>35,00 mill. €</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>Cody Gakpo</v>
+        <v>Matheus Nunes</v>
       </c>
       <c r="B100" t="str">
         <v>26</v>
       </c>
       <c r="C100" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Mediocentro</v>
       </c>
       <c r="D100" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/434675-1682690965.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/601883-1693561106.jpg?lm=1</v>
       </c>
       <c r="E100" t="str">
-        <v>Países Bajos</v>
+        <v>Portugal</v>
       </c>
       <c r="F100" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
       </c>
       <c r="G100" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
       </c>
       <c r="H100" t="str">
-        <v>Liverpool FC</v>
+        <v>Manchester City</v>
       </c>
       <c r="I100" t="str">
-        <v>70,00 mill. €</v>
+        <v>55,00 mill. €</v>
       </c>
       <c r="J100" t="str">
-        <v>Togo</v>
+        <v>30/05/2025</v>
       </c>
       <c r="K100" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/168.png?lm=1520611569</v>
+        <v>35,00 mill. €</v>
       </c>
       <c r="L100" t="str">
-        <v>70,00 mill. €</v>
+        <v>Brasil</v>
       </c>
       <c r="M100" t="str">
-        <v>30/05/2025</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/26.png?lm=1520611569</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>Luis Díaz</v>
+        <v>Riccardo Calafiori</v>
       </c>
       <c r="B101" t="str">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C101" t="str">
-        <v>Extremo izquierdo</v>
+        <v>Lateral izquierdo</v>
       </c>
       <c r="D101" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/480692-1697903145.jpg?lm=1</v>
+        <v>https://img.a.transfermarkt.technology/portrait/medium/502821-1727382174.jpg?lm=1</v>
       </c>
       <c r="E101" t="str">
-        <v>Colombia</v>
+        <v>Italia</v>
       </c>
       <c r="F101" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/83.png?lm=1520611569</v>
+        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
       </c>
       <c r="G101" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/31.png?lm=1727873452</v>
+        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
       </c>
       <c r="H101" t="str">
-        <v>Liverpool FC</v>
+        <v>Arsenal FC</v>
       </c>
       <c r="I101" t="str">
-        <v>70,00 mill. €</v>
-      </c>
-      <c r="L101" t="str">
-        <v>85,00 mill. €</v>
-      </c>
-      <c r="M101" t="str">
-        <v>30/05/2025</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="str">
-        <v>Rúben Dias</v>
-      </c>
-      <c r="B102" t="str">
-        <v>28</v>
-      </c>
-      <c r="C102" t="str">
-        <v>Defensa central</v>
-      </c>
-      <c r="D102" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/258004-1684921271.jpg?lm=1</v>
-      </c>
-      <c r="E102" t="str">
-        <v>Portugal</v>
-      </c>
-      <c r="F102" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/136.png?lm=1520611569</v>
-      </c>
-      <c r="G102" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
-      </c>
-      <c r="H102" t="str">
-        <v>Manchester City</v>
-      </c>
-      <c r="I102" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="L102" t="str">
-        <v>80,00 mill. €</v>
-      </c>
-      <c r="M102" t="str">
-        <v>30/05/2025</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="str">
-        <v>Kai Havertz</v>
-      </c>
-      <c r="B103" t="str">
-        <v>26</v>
-      </c>
-      <c r="C103" t="str">
-        <v>Delantero centro</v>
-      </c>
-      <c r="D103" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/309400-1683903902.jpg?lm=1</v>
-      </c>
-      <c r="E103" t="str">
-        <v>Alemania</v>
-      </c>
-      <c r="F103" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/40.png?lm=1520612525</v>
-      </c>
-      <c r="G103" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/11.png?lm=1489787850</v>
-      </c>
-      <c r="H103" t="str">
-        <v>Arsenal FC</v>
-      </c>
-      <c r="I103" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="L103" t="str">
-        <v>90,00 mill. €</v>
-      </c>
-      <c r="M103" t="str">
-        <v>30/05/2025</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="str">
-        <v>Anthony Gordon</v>
-      </c>
-      <c r="B104" t="str">
-        <v>24</v>
-      </c>
-      <c r="C104" t="str">
-        <v>Extremo izquierdo</v>
-      </c>
-      <c r="D104" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/503733-1660588736.jpg?lm=1</v>
-      </c>
-      <c r="E104" t="str">
-        <v>Inglaterra</v>
-      </c>
-      <c r="F104" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/189.png?lm=1520611569</v>
-      </c>
-      <c r="G104" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
-      </c>
-      <c r="H104" t="str">
-        <v>Newcastle United</v>
-      </c>
-      <c r="I104" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="L104" t="str">
-        <v>65,00 mill. €</v>
-      </c>
-      <c r="M104" t="str">
-        <v>30/05/2025</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="str">
-        <v>Sandro Tonali</v>
-      </c>
-      <c r="B105" t="str">
-        <v>25</v>
-      </c>
-      <c r="C105" t="str">
-        <v>Mediocentro</v>
-      </c>
-      <c r="D105" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/397033-1688389270.jpg?lm=1</v>
-      </c>
-      <c r="E105" t="str">
-        <v>Italia</v>
-      </c>
-      <c r="F105" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/75.png?lm=1520611569</v>
-      </c>
-      <c r="G105" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/762.png?lm=1472921161</v>
-      </c>
-      <c r="H105" t="str">
-        <v>Newcastle United</v>
-      </c>
-      <c r="I105" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="L105" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="M105" t="str">
-        <v>30/05/2025</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="str">
-        <v>Tijjani Reijnders</v>
-      </c>
-      <c r="B106" t="str">
-        <v>26</v>
-      </c>
-      <c r="C106" t="str">
-        <v>Mediocentro</v>
-      </c>
-      <c r="D106" t="str">
-        <v>https://img.a.transfermarkt.technology/portrait/medium/460939-1676466080.jpg?lm=1</v>
-      </c>
-      <c r="E106" t="str">
-        <v>Países Bajos</v>
-      </c>
-      <c r="F106" t="str">
-        <v>https://tmssl.akamaized.net//images/flagge/verysmall/122.png?lm=1520611569</v>
-      </c>
-      <c r="G106" t="str">
-        <v>https://tmssl.akamaized.net//images/wappen/verysmall/281.png?lm=1467356331</v>
-      </c>
-      <c r="H106" t="str">
-        <v>Manchester City</v>
-      </c>
-      <c r="I106" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="L106" t="str">
-        <v>60,00 mill. €</v>
-      </c>
-      <c r="M106" t="str">
-        <v>17/06/2025</v>
+        <v>45,00 mill. €</v>
+      </c>
+      <c r="J101" t="str">
+        <v>30/05/2025</v>
+      </c>
+      <c r="K101" t="str">
+        <v>35,00 mill. €</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M106"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M101"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>